<commit_message>
finalised minium requirement dialog manager
tested
</commit_message>
<xml_diff>
--- a/doc/cnc_troubleshooting.xlsx
+++ b/doc/cnc_troubleshooting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -29,6 +29,27 @@
   </si>
   <si>
     <t>Unnamed: 0.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1</t>
   </si>
   <si>
     <t>Parts</t>
@@ -455,13 +476,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +510,29 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -509,20 +551,41 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -541,20 +604,41 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -573,20 +657,41 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" t="s">
         <v>17</v>
       </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -605,52 +710,94 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" t="s">
         <v>18</v>
       </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -669,272 +816,461 @@
       <c r="F7">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>9</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" t="s">
         <v>19</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="P12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>11</v>
+      </c>
+      <c r="J13">
+        <v>11</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="M13">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" t="s">
+        <v>19</v>
+      </c>
+      <c r="P13" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <v>12</v>
+      </c>
+      <c r="J14">
+        <v>12</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14" t="s">
+        <v>16</v>
+      </c>
+      <c r="O14" t="s">
         <v>20</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="P14" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>13</v>
+      </c>
+      <c r="J15">
+        <v>13</v>
+      </c>
+      <c r="K15">
+        <v>13</v>
+      </c>
+      <c r="L15">
+        <v>13</v>
+      </c>
+      <c r="M15">
+        <v>13</v>
+      </c>
+      <c r="N15" t="s">
+        <v>16</v>
+      </c>
+      <c r="O15" t="s">
         <v>21</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>9</v>
-      </c>
-      <c r="F11">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>11</v>
-      </c>
-      <c r="D13">
-        <v>11</v>
-      </c>
-      <c r="E13">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14">
-        <v>12</v>
-      </c>
-      <c r="E14">
-        <v>12</v>
-      </c>
-      <c r="F14">
-        <v>12</v>
-      </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>13</v>
-      </c>
-      <c r="D15">
-        <v>13</v>
-      </c>
-      <c r="E15">
-        <v>13</v>
-      </c>
-      <c r="F15">
-        <v>13</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15">
+      <c r="P15" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15">
         <v>0</v>
       </c>
     </row>

</xml_diff>